<commit_message>
Updates to ASWCS FFBD/IDEF0 and context diagrams.
FFBD/IDEF0 diagrams are contained in a Visio file; (incomplete) context diagrams are in an Excel file.
</commit_message>
<xml_diff>
--- a/ASWCS_TJG_Context_Diagrams.xlsx
+++ b/ASWCS_TJG_Context_Diagrams.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18285" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18285" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Pilot Vessel Out of Port" sheetId="1" r:id="rId1"/>
@@ -31,49 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>Mow Lawn</t>
-  </si>
-  <si>
-    <t>Mower
-Mower Operator</t>
-  </si>
-  <si>
-    <t>Grass Clippings
-Hydrocarbons</t>
-  </si>
-  <si>
-    <t>Weather
-Availability of Power</t>
-  </si>
-  <si>
-    <t>Fuel
-Grass to be Mown</t>
-  </si>
-  <si>
-    <t>Build Small PCB</t>
-  </si>
-  <si>
-    <t>PCB/PerfBoard
-Components
-Solder</t>
-  </si>
-  <si>
-    <t>Completed PCB
-Clipped Leads</t>
-  </si>
-  <si>
-    <t>Technician
-Soldering Iron/Station
-Wet Sponge</t>
-  </si>
-  <si>
-    <t>Power Availability
-Solder Fume Extraction</t>
   </si>
   <si>
     <t>Pilot Vessel Out of Port</t>
@@ -143,15 +103,95 @@
     <t>Plastic Waste on Transport Vessel</t>
   </si>
   <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Generator Set
+Waste Transfer Controller
+Weight Sensor
+Volumetric Sensor</t>
+  </si>
+  <si>
     <t>Plastic Waste on Collector
-220 VAC, 50A Electrical Power</t>
+220 VAC, 50A Electrical Power
+Weight Sensor Data
+Volumetric Sensor Data</t>
+  </si>
+  <si>
+    <t>Recycling Center Personnel
+Waste Transfer Controller
+Weight Sensor
+Volumetric Sensor</t>
+  </si>
+  <si>
+    <t>Transfer Waste from Transport Vessel to Recycling Facility</t>
+  </si>
+  <si>
+    <t>Fuel
+Weight Sensor Data
+Volumetric Sensor Data
+Plastic Waste</t>
+  </si>
+  <si>
+    <t>Plastic Waste in Recycling Facility</t>
+  </si>
+  <si>
+    <r>
+      <t>Full H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Tanks</t>
+    </r>
+  </si>
+  <si>
+    <t>Harbor Pilot
+Bunker Facility Operator</t>
+  </si>
+  <si>
+    <t>Dock at Bunker Pier and Refuel Transport Vessel</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  Bunker Fuel (H</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>?)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -160,6 +200,11 @@
     <font>
       <vertAlign val="subscript"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -199,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -214,6 +259,22 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -498,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
@@ -509,23 +570,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -557,7 +618,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -567,23 +628,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -628,23 +689,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -675,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -685,21 +746,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
+      <c r="A2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5"/>
+      <c r="A3" s="6"/>
+      <c r="B3" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -726,7 +795,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -735,25 +804,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>4</v>
+      <c r="B1" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
+      <c r="A2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A3" s="6"/>
+      <c r="B3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -779,7 +850,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B4" sqref="A1:XFD1048576"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -788,25 +859,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -832,7 +893,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -842,23 +903,23 @@
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -885,7 +946,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -894,25 +955,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
+      <c r="B3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:3" ht="76.900000000000006" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>